<commit_message>
updated PPIT and ITW assignments
</commit_message>
<xml_diff>
--- a/ITW/u3149399/P2-u3149399-SalesReports.xlsx
+++ b/ITW/u3149399/P2-u3149399-SalesReports.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27106"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27106"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -15,12 +15,16 @@
     <sheet name="Quarterly Sales Summary" sheetId="1" r:id="rId1"/>
     <sheet name="Bonuses" sheetId="2" r:id="rId2"/>
     <sheet name="Sales Projections" sheetId="4" r:id="rId3"/>
-    <sheet name="Trips" sheetId="7" r:id="rId4"/>
+    <sheet name="Pivot Table" sheetId="8" r:id="rId4"/>
+    <sheet name="Trips" sheetId="7" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Bonuses!$A$4:$H$17</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
+  <pivotCaches>
+    <pivotCache cacheId="5" r:id="rId6"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -33,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="71">
   <si>
     <t>Total</t>
   </si>
@@ -232,21 +236,34 @@
   <si>
     <t>Their average profit per trip</t>
   </si>
+  <si>
+    <t>Emily Deschanels, Q4</t>
+  </si>
+  <si>
+    <t>Column Labels</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Sum of Profit</t>
+  </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="9">
+  <numFmts count="7">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0"/>
     <numFmt numFmtId="167" formatCode="_-[$$-C09]* #,##0.00_-;\-[$$-C09]* #,##0.00_-;_-[$$-C09]* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="168" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -305,7 +322,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color indexed="206"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -324,7 +341,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -379,8 +396,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -396,12 +428,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -437,26 +468,47 @@
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" xfId="14" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="9" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="18" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="17" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="18"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="17"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="13" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="17" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="16" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="18" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="17" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="13"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="16" applyFont="1"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="16" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="15" applyFont="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="15" applyFont="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="13" applyFill="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="17" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="16" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="14" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="3" xfId="17" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="16" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="15" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="15"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="15" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="15" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" xfId="14" applyFont="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="15" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="11" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -469,39 +521,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="10" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" xfId="14" applyFont="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="14" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="3" xfId="18" applyNumberFormat="1"/>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" xfId="14" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="15" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="15" applyNumberFormat="1"/>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="3" xfId="18" applyNumberFormat="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="3" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="17" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="5" fillId="0" borderId="3" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="18">
     <cellStyle name="5poRJfl+ZUAkAS/y55FTKjP2V4R9Xff8nrFfXKHIidA=-~DyJpIdC918Oc2CKKuumpPw==" xfId="10"/>
     <cellStyle name="5t47kWWunSzTCk1qkInIM9eYIGYLTxfZ7EEg1TLNvM4=-~u4zsNRx4wvy/FmHi9eWYbQ==" xfId="6"/>
     <cellStyle name="6s5SMWIpcuoqy3L3CIsYmq35hVHLmXdCLC6DkB1+bhI=-~Rj+ExFvfEGkif5XTceoN6w==" xfId="5"/>
     <cellStyle name="Agg4hU8OSPnPZOLCXW3ZgSWrv1zKfezZ76dWV8T4mHs=-~yYXjbT5LhV/XzzqmfGrNWw==" xfId="2"/>
     <cellStyle name="C+nOzAM2cDCptqLFnt/A03jKZSNR54D7k0++S/SAfqg=-~B+04lu6Lty4sXY9c3r4guw==" xfId="4"/>
     <cellStyle name="cmytORPWR7LIeEI5FPZFXNFloiU1XmMOAsT+u9oIoyk=-~+4wdbmbwoI0TlrQQW93Hhw==" xfId="8"/>
-    <cellStyle name="Comma [0]" xfId="15" builtinId="6"/>
-    <cellStyle name="Currency" xfId="16" builtinId="4"/>
+    <cellStyle name="Currency" xfId="15" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="14" builtinId="7"/>
     <cellStyle name="Dgz22PdKSkfNaPGCdRA31rxYSssO+ShLve/ofKCrbuQ=-~W1+GB9ISLxDDUHHvkmmfLg==" xfId="3"/>
     <cellStyle name="DNkQiQOOro3gnXXaMWm2Hdzp4xJJfS1C/+zToIdqLss=-~aA/KQKIp7CfIKO034u15dQ==" xfId="1"/>
@@ -510,11 +543,102 @@
     <cellStyle name="IlMEMBVqLO4OKQv8HrrcQNjfi3yuERbqvSo+IFdydlg=-~3pnlt15Z0ODJ5iTjvKIJxQ==" xfId="7"/>
     <cellStyle name="iRKU8G5OdV69kghBVfjk5q0bkBLkgow7mATqkTWl0lM=-~UCmDN39TD5BDt/zqjKdSnQ==" xfId="9"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="17" builtinId="5"/>
+    <cellStyle name="Percent" xfId="16" builtinId="5"/>
     <cellStyle name="Title" xfId="11" builtinId="15"/>
-    <cellStyle name="Total" xfId="18" builtinId="25"/>
+    <cellStyle name="Total" xfId="17" builtinId="25"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="6">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -533,9 +657,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1013,11 +1134,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="2127812992"/>
-        <c:axId val="2127816560"/>
+        <c:axId val="2123763680"/>
+        <c:axId val="2123768800"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2127812992"/>
+        <c:axId val="2123763680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1113,7 +1234,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2127816560"/>
+        <c:crossAx val="2123768800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1121,7 +1242,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2127816560"/>
+        <c:axId val="2123768800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1161,7 +1282,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>SALE</a:t>
+                  <a:t>SALES</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1225,7 +1346,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2127812992"/>
+        <c:crossAx val="2123763680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1527,7 +1648,7 @@
             <c:numRef>
               <c:f>Bonuses!$C$5:$C$17</c:f>
               <c:numCache>
-                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:formatCode>_-"$"* #,##0.00_-;\-"$"* #,##0.00_-;_-"$"* "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>18638.33333333333</c:v>
@@ -1694,7 +1815,7 @@
             <c:numRef>
               <c:f>Bonuses!$D$5:$D$17</c:f>
               <c:numCache>
-                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:formatCode>_-"$"* #,##0.00_-;\-"$"* #,##0.00_-;_-"$"* "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>24229.83333333333</c:v>
@@ -1861,7 +1982,7 @@
             <c:numRef>
               <c:f>Bonuses!$E$5:$E$17</c:f>
               <c:numCache>
-                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:formatCode>_-"$"* #,##0.00_-;\-"$"* #,##0.00_-;_-"$"* "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>25586.704</c:v>
@@ -2028,7 +2149,7 @@
             <c:numRef>
               <c:f>Bonuses!$F$5:$F$17</c:f>
               <c:numCache>
-                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:formatCode>_-"$"* #,##0.00_-;\-"$"* #,##0.00_-;_-"$"* "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>17398.95872</c:v>
@@ -2083,11 +2204,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-24"/>
-        <c:axId val="-2090776272"/>
-        <c:axId val="-2090178576"/>
+        <c:axId val="-2137741104"/>
+        <c:axId val="-2117608704"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2090776272"/>
+        <c:axId val="-2137741104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2113,7 +2234,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>SALE REPRESENTATIVE</a:t>
+                  <a:t>SALE REPRESENTATIVEs</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -2183,7 +2304,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2090178576"/>
+        <c:crossAx val="-2117608704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2191,7 +2312,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2090178576"/>
+        <c:axId val="-2117608704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2231,7 +2352,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>SALE</a:t>
+                  <a:t>SALEs</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -2294,7 +2415,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2090776272"/>
+        <c:crossAx val="-2137741104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3496,16 +3617,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>476250</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>44450</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>482600</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3579,6 +3700,2041 @@
     <xdr:clientData/>
   </xdr:oneCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Tenzin Dendup" refreshedDate="42849.651619328703" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="208">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A9:G217" sheet="Trips"/>
+  </cacheSource>
+  <cacheFields count="7">
+    <cacheField name="Sales Representative" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Region" numFmtId="0">
+      <sharedItems count="3">
+        <s v="NZ"/>
+        <s v="AUS"/>
+        <s v="Intl"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Quarter" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="4" count="4">
+        <n v="2"/>
+        <n v="1"/>
+        <n v="4"/>
+        <n v="3"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Network" numFmtId="0">
+      <sharedItems count="5">
+        <s v="Classic Movie and TV Networks"/>
+        <s v="International Networks"/>
+        <s v="Film Entertainment Networks"/>
+        <s v="Young Adult Networks"/>
+        <s v="Sports Networks"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Sales" numFmtId="164">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="1008.28" maxValue="4994.09"/>
+    </cacheField>
+    <cacheField name="Trip expenditures" numFmtId="167">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="218.52" maxValue="996.29"/>
+    </cacheField>
+    <cacheField name="Profit" numFmtId="164">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="90.459999999999923" maxValue="4649.58"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="208">
+  <r>
+    <s v="Lisa Steinberg"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="2487.19"/>
+    <n v="560.66999999999996"/>
+    <n v="1926.52"/>
+  </r>
+  <r>
+    <s v="Catherine Williams"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="3970.28"/>
+    <n v="356.85"/>
+    <n v="3613.4300000000003"/>
+  </r>
+  <r>
+    <s v="Emily Deschanels"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="2609.08"/>
+    <n v="936.3"/>
+    <n v="1672.78"/>
+  </r>
+  <r>
+    <s v="Lisa Vanderbeck"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="1323.57"/>
+    <n v="386.15"/>
+    <n v="937.42"/>
+  </r>
+  <r>
+    <s v="Lori Rukstad"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="2086.37"/>
+    <n v="341.91"/>
+    <n v="1744.4599999999998"/>
+  </r>
+  <r>
+    <s v="Michael Roberts"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="3"/>
+    <n v="4619.3100000000004"/>
+    <n v="275.86"/>
+    <n v="4343.4500000000007"/>
+  </r>
+  <r>
+    <s v="Peter Little"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="4329.51"/>
+    <n v="365.78"/>
+    <n v="3963.7300000000005"/>
+  </r>
+  <r>
+    <s v="Robert Mitchells"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="4891.83"/>
+    <n v="939.82"/>
+    <n v="3952.0099999999998"/>
+  </r>
+  <r>
+    <s v="Ryan Lawton"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="3"/>
+    <n v="2516.42"/>
+    <n v="337.17"/>
+    <n v="2179.25"/>
+  </r>
+  <r>
+    <s v="Samuel Kackowski"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="1500.18"/>
+    <n v="933.89"/>
+    <n v="566.29000000000008"/>
+  </r>
+  <r>
+    <s v="Sydney Hood"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="1421.19"/>
+    <n v="573.69000000000005"/>
+    <n v="847.5"/>
+  </r>
+  <r>
+    <s v="Ted Harris"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="3"/>
+    <n v="1568.21"/>
+    <n v="799.52"/>
+    <n v="768.69"/>
+  </r>
+  <r>
+    <s v="Trey Wingo"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="3"/>
+    <n v="3100.23"/>
+    <n v="397.43"/>
+    <n v="2702.8"/>
+  </r>
+  <r>
+    <s v="Lisa Steinberg"/>
+    <x v="0"/>
+    <x v="3"/>
+    <x v="2"/>
+    <n v="4385.97"/>
+    <n v="853.51"/>
+    <n v="3532.46"/>
+  </r>
+  <r>
+    <s v="Catherine Williams"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="3745.01"/>
+    <n v="785.81"/>
+    <n v="2959.2000000000003"/>
+  </r>
+  <r>
+    <s v="Emily Deschanels"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="1452.18"/>
+    <n v="608.91"/>
+    <n v="843.2700000000001"/>
+  </r>
+  <r>
+    <s v="Lisa Vanderbeck"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="3948.69"/>
+    <n v="926.91"/>
+    <n v="3021.78"/>
+  </r>
+  <r>
+    <s v="Lori Rukstad"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="4830.67"/>
+    <n v="362.91"/>
+    <n v="4467.76"/>
+  </r>
+  <r>
+    <s v="Michael Roberts"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="3"/>
+    <n v="2598.16"/>
+    <n v="340.36"/>
+    <n v="2257.7999999999997"/>
+  </r>
+  <r>
+    <s v="Peter Little"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="4527.92"/>
+    <n v="891.72"/>
+    <n v="3636.2"/>
+  </r>
+  <r>
+    <s v="Robert Mitchells"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="3711.56"/>
+    <n v="960.6"/>
+    <n v="2750.96"/>
+  </r>
+  <r>
+    <s v="Ryan Lawton"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="4"/>
+    <n v="1860.26"/>
+    <n v="226.65"/>
+    <n v="1633.61"/>
+  </r>
+  <r>
+    <s v="Samuel Kackowski"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="3306.77"/>
+    <n v="325.77999999999997"/>
+    <n v="2980.99"/>
+  </r>
+  <r>
+    <s v="Sydney Hood"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="4"/>
+    <n v="2403.91"/>
+    <n v="690.18"/>
+    <n v="1713.73"/>
+  </r>
+  <r>
+    <s v="Ted Harris"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="1602.8"/>
+    <n v="879.27"/>
+    <n v="723.53"/>
+  </r>
+  <r>
+    <s v="Trey Wingo"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="3811.64"/>
+    <n v="286.92"/>
+    <n v="3524.72"/>
+  </r>
+  <r>
+    <s v="Lisa Steinberg"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="2994.44"/>
+    <n v="746.55"/>
+    <n v="2247.8900000000003"/>
+  </r>
+  <r>
+    <s v="Catherine Williams"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="2920.73"/>
+    <n v="909.01"/>
+    <n v="2011.72"/>
+  </r>
+  <r>
+    <s v="Emily Deschanels"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="4841.88"/>
+    <n v="664.92"/>
+    <n v="4176.96"/>
+  </r>
+  <r>
+    <s v="Lisa Vanderbeck"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="1109.1099999999999"/>
+    <n v="628.04"/>
+    <n v="481.06999999999994"/>
+  </r>
+  <r>
+    <s v="Lori Rukstad"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="4"/>
+    <n v="3648.19"/>
+    <n v="987.94"/>
+    <n v="2660.25"/>
+  </r>
+  <r>
+    <s v="Michael Roberts"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="1570.65"/>
+    <n v="371.84"/>
+    <n v="1198.8100000000002"/>
+  </r>
+  <r>
+    <s v="Peter Little"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="3"/>
+    <n v="4210.09"/>
+    <n v="697.21"/>
+    <n v="3512.88"/>
+  </r>
+  <r>
+    <s v="Robert Mitchells"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="4"/>
+    <n v="3588.41"/>
+    <n v="299.20999999999998"/>
+    <n v="3289.2"/>
+  </r>
+  <r>
+    <s v="Ryan Lawton"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="4760.25"/>
+    <n v="507.06"/>
+    <n v="4253.1899999999996"/>
+  </r>
+  <r>
+    <s v="Samuel Kackowski"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="3"/>
+    <n v="4167.92"/>
+    <n v="334.68"/>
+    <n v="3833.2400000000002"/>
+  </r>
+  <r>
+    <s v="Sydney Hood"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="4992.97"/>
+    <n v="728.28"/>
+    <n v="4264.6900000000005"/>
+  </r>
+  <r>
+    <s v="Ted Harris"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="1080.81"/>
+    <n v="857.9"/>
+    <n v="222.90999999999997"/>
+  </r>
+  <r>
+    <s v="Trey Wingo"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="1640.21"/>
+    <n v="513.09"/>
+    <n v="1127.1199999999999"/>
+  </r>
+  <r>
+    <s v="Lisa Steinberg"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="3792.83"/>
+    <n v="313.22000000000003"/>
+    <n v="3479.6099999999997"/>
+  </r>
+  <r>
+    <s v="Catherine Williams"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="2651.4"/>
+    <n v="926.31"/>
+    <n v="1725.0900000000001"/>
+  </r>
+  <r>
+    <s v="Emily Deschanels"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="4"/>
+    <n v="1631.16"/>
+    <n v="839.62"/>
+    <n v="791.54000000000008"/>
+  </r>
+  <r>
+    <s v="Lisa Vanderbeck"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="4"/>
+    <n v="1426.74"/>
+    <n v="914.4"/>
+    <n v="512.34"/>
+  </r>
+  <r>
+    <s v="Lori Rukstad"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="3474.67"/>
+    <n v="897.16"/>
+    <n v="2577.5100000000002"/>
+  </r>
+  <r>
+    <s v="Michael Roberts"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="3"/>
+    <n v="4938.4399999999996"/>
+    <n v="800.74"/>
+    <n v="4137.7"/>
+  </r>
+  <r>
+    <s v="Peter Little"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="2481.2399999999998"/>
+    <n v="885.45"/>
+    <n v="1595.7899999999997"/>
+  </r>
+  <r>
+    <s v="Robert Mitchells"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="4163.2299999999996"/>
+    <n v="463.27"/>
+    <n v="3699.9599999999996"/>
+  </r>
+  <r>
+    <s v="Ryan Lawton"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="1399.48"/>
+    <n v="593.85"/>
+    <n v="805.63"/>
+  </r>
+  <r>
+    <s v="Samuel Kackowski"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="1594.71"/>
+    <n v="722.65"/>
+    <n v="872.06000000000006"/>
+  </r>
+  <r>
+    <s v="Sydney Hood"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="3012.62"/>
+    <n v="223.77"/>
+    <n v="2788.85"/>
+  </r>
+  <r>
+    <s v="Ted Harris"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="3289.86"/>
+    <n v="633.75"/>
+    <n v="2656.11"/>
+  </r>
+  <r>
+    <s v="Trey Wingo"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="1106.45"/>
+    <n v="885.88"/>
+    <n v="220.57000000000005"/>
+  </r>
+  <r>
+    <s v="Lisa Steinberg"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="3088.06"/>
+    <n v="439.45"/>
+    <n v="2648.61"/>
+  </r>
+  <r>
+    <s v="Catherine Williams"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="1546.7"/>
+    <n v="314.13"/>
+    <n v="1232.5700000000002"/>
+  </r>
+  <r>
+    <s v="Emily Deschanels"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="2730.3"/>
+    <n v="704.72"/>
+    <n v="2025.5800000000002"/>
+  </r>
+  <r>
+    <s v="Lisa Vanderbeck"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="3115.91"/>
+    <n v="695.56"/>
+    <n v="2420.35"/>
+  </r>
+  <r>
+    <s v="Lori Rukstad"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="4664.22"/>
+    <n v="565.66"/>
+    <n v="4098.5600000000004"/>
+  </r>
+  <r>
+    <s v="Michael Roberts"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="4"/>
+    <n v="1008.28"/>
+    <n v="572.46"/>
+    <n v="435.81999999999994"/>
+  </r>
+  <r>
+    <s v="Peter Little"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="4"/>
+    <n v="3733.88"/>
+    <n v="784.38"/>
+    <n v="2949.5"/>
+  </r>
+  <r>
+    <s v="Robert Mitchells"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="1502.58"/>
+    <n v="967.44"/>
+    <n v="535.13999999999987"/>
+  </r>
+  <r>
+    <s v="Ryan Lawton"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="4140.57"/>
+    <n v="908.27"/>
+    <n v="3232.2999999999997"/>
+  </r>
+  <r>
+    <s v="Samuel Kackowski"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="1495.34"/>
+    <n v="956.46"/>
+    <n v="538.87999999999988"/>
+  </r>
+  <r>
+    <s v="Sydney Hood"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="4"/>
+    <n v="2008.03"/>
+    <n v="451.6"/>
+    <n v="1556.4299999999998"/>
+  </r>
+  <r>
+    <s v="Ted Harris"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="2"/>
+    <n v="1367.34"/>
+    <n v="254.1"/>
+    <n v="1113.24"/>
+  </r>
+  <r>
+    <s v="Trey Wingo"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="4"/>
+    <n v="3095.29"/>
+    <n v="867.38"/>
+    <n v="2227.91"/>
+  </r>
+  <r>
+    <s v="Lisa Steinberg"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="4534.05"/>
+    <n v="532.67999999999995"/>
+    <n v="4001.3700000000003"/>
+  </r>
+  <r>
+    <s v="Catherine Williams"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="1297.51"/>
+    <n v="757.61"/>
+    <n v="539.9"/>
+  </r>
+  <r>
+    <s v="Emily Deschanels"/>
+    <x v="0"/>
+    <x v="3"/>
+    <x v="1"/>
+    <n v="2917.65"/>
+    <n v="576.54999999999995"/>
+    <n v="2341.1000000000004"/>
+  </r>
+  <r>
+    <s v="Lisa Vanderbeck"/>
+    <x v="0"/>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="4772.63"/>
+    <n v="655.95"/>
+    <n v="4116.68"/>
+  </r>
+  <r>
+    <s v="Lori Rukstad"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="3509.95"/>
+    <n v="554.97"/>
+    <n v="2954.9799999999996"/>
+  </r>
+  <r>
+    <s v="Michael Roberts"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="4"/>
+    <n v="2234.5700000000002"/>
+    <n v="357.51"/>
+    <n v="1877.0600000000002"/>
+  </r>
+  <r>
+    <s v="Peter Little"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="2767.82"/>
+    <n v="695.57"/>
+    <n v="2072.25"/>
+  </r>
+  <r>
+    <s v="Robert Mitchells"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="3663.43"/>
+    <n v="537.88"/>
+    <n v="3125.5499999999997"/>
+  </r>
+  <r>
+    <s v="Ryan Lawton"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="1680.27"/>
+    <n v="497.17"/>
+    <n v="1183.0999999999999"/>
+  </r>
+  <r>
+    <s v="Samuel Kackowski"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="4444.07"/>
+    <n v="960.04"/>
+    <n v="3484.0299999999997"/>
+  </r>
+  <r>
+    <s v="Sydney Hood"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="3"/>
+    <n v="4994.09"/>
+    <n v="900.7"/>
+    <n v="4093.3900000000003"/>
+  </r>
+  <r>
+    <s v="Ted Harris"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="2012.31"/>
+    <n v="991.12"/>
+    <n v="1021.1899999999999"/>
+  </r>
+  <r>
+    <s v="Trey Wingo"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="2"/>
+    <n v="4026.56"/>
+    <n v="716.1"/>
+    <n v="3310.46"/>
+  </r>
+  <r>
+    <s v="Lisa Steinberg"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="1583.01"/>
+    <n v="369.64"/>
+    <n v="1213.3699999999999"/>
+  </r>
+  <r>
+    <s v="Catherine Williams"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="1"/>
+    <n v="4370.66"/>
+    <n v="668.44"/>
+    <n v="3702.22"/>
+  </r>
+  <r>
+    <s v="Emily Deschanels"/>
+    <x v="0"/>
+    <x v="3"/>
+    <x v="4"/>
+    <n v="4222.38"/>
+    <n v="689.51"/>
+    <n v="3532.87"/>
+  </r>
+  <r>
+    <s v="Lisa Vanderbeck"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="1302.95"/>
+    <n v="428.31"/>
+    <n v="874.6400000000001"/>
+  </r>
+  <r>
+    <s v="Lori Rukstad"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="4172.4799999999996"/>
+    <n v="996.29"/>
+    <n v="3176.1899999999996"/>
+  </r>
+  <r>
+    <s v="Michael Roberts"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="3462.63"/>
+    <n v="811.65"/>
+    <n v="2650.98"/>
+  </r>
+  <r>
+    <s v="Peter Little"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="4"/>
+    <n v="3441.57"/>
+    <n v="290.27999999999997"/>
+    <n v="3151.29"/>
+  </r>
+  <r>
+    <s v="Robert Mitchells"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="4"/>
+    <n v="3676.78"/>
+    <n v="651.39"/>
+    <n v="3025.3900000000003"/>
+  </r>
+  <r>
+    <s v="Ryan Lawton"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="3840.65"/>
+    <n v="741.35"/>
+    <n v="3099.3"/>
+  </r>
+  <r>
+    <s v="Samuel Kackowski"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="1105.76"/>
+    <n v="775.65"/>
+    <n v="330.11"/>
+  </r>
+  <r>
+    <s v="Sydney Hood"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="2697.61"/>
+    <n v="237.37"/>
+    <n v="2460.2400000000002"/>
+  </r>
+  <r>
+    <s v="Ted Harris"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="1206.04"/>
+    <n v="238.39"/>
+    <n v="967.65"/>
+  </r>
+  <r>
+    <s v="Trey Wingo"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="4"/>
+    <n v="2997.38"/>
+    <n v="500.19"/>
+    <n v="2497.19"/>
+  </r>
+  <r>
+    <s v="Lisa Steinberg"/>
+    <x v="0"/>
+    <x v="3"/>
+    <x v="1"/>
+    <n v="1357.52"/>
+    <n v="717.29"/>
+    <n v="640.23"/>
+  </r>
+  <r>
+    <s v="Catherine Williams"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="4653.8599999999997"/>
+    <n v="879.65"/>
+    <n v="3774.2099999999996"/>
+  </r>
+  <r>
+    <s v="Emily Deschanels"/>
+    <x v="0"/>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="4493.55"/>
+    <n v="726.41"/>
+    <n v="3767.1400000000003"/>
+  </r>
+  <r>
+    <s v="Lisa Vanderbeck"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="4833.4799999999996"/>
+    <n v="246.38"/>
+    <n v="4587.0999999999995"/>
+  </r>
+  <r>
+    <s v="Lori Rukstad"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="3922.33"/>
+    <n v="517.67999999999995"/>
+    <n v="3404.65"/>
+  </r>
+  <r>
+    <s v="Michael Roberts"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="2"/>
+    <n v="4941.88"/>
+    <n v="692.86"/>
+    <n v="4249.0200000000004"/>
+  </r>
+  <r>
+    <s v="Peter Little"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="4"/>
+    <n v="4182.9399999999996"/>
+    <n v="915.73"/>
+    <n v="3267.2099999999996"/>
+  </r>
+  <r>
+    <s v="Robert Mitchells"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="1211.0999999999999"/>
+    <n v="590.13"/>
+    <n v="620.96999999999991"/>
+  </r>
+  <r>
+    <s v="Ryan Lawton"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="2748.94"/>
+    <n v="630.53"/>
+    <n v="2118.41"/>
+  </r>
+  <r>
+    <s v="Samuel Kackowski"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="2850.09"/>
+    <n v="687.6"/>
+    <n v="2162.4900000000002"/>
+  </r>
+  <r>
+    <s v="Sydney Hood"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="4799.38"/>
+    <n v="905.96"/>
+    <n v="3893.42"/>
+  </r>
+  <r>
+    <s v="Ted Harris"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="4881.21"/>
+    <n v="231.63"/>
+    <n v="4649.58"/>
+  </r>
+  <r>
+    <s v="Trey Wingo"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="1351.27"/>
+    <n v="604.28"/>
+    <n v="746.99"/>
+  </r>
+  <r>
+    <s v="Lisa Steinberg"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="2627.45"/>
+    <n v="756.27"/>
+    <n v="1871.1799999999998"/>
+  </r>
+  <r>
+    <s v="Catherine Williams"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="3"/>
+    <n v="4880.53"/>
+    <n v="851.42"/>
+    <n v="4029.1099999999997"/>
+  </r>
+  <r>
+    <s v="Emily Deschanels"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="2792.08"/>
+    <n v="741.98"/>
+    <n v="2050.1"/>
+  </r>
+  <r>
+    <s v="Lisa Vanderbeck"/>
+    <x v="0"/>
+    <x v="3"/>
+    <x v="1"/>
+    <n v="3759.22"/>
+    <n v="398.84"/>
+    <n v="3360.3799999999997"/>
+  </r>
+  <r>
+    <s v="Lori Rukstad"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="1240.76"/>
+    <n v="437.01"/>
+    <n v="803.75"/>
+  </r>
+  <r>
+    <s v="Michael Roberts"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="3673.08"/>
+    <n v="515.35"/>
+    <n v="3157.73"/>
+  </r>
+  <r>
+    <s v="Peter Little"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="1365.53"/>
+    <n v="279.79000000000002"/>
+    <n v="1085.74"/>
+  </r>
+  <r>
+    <s v="Robert Mitchells"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="4"/>
+    <n v="4634.09"/>
+    <n v="362.53"/>
+    <n v="4271.5600000000004"/>
+  </r>
+  <r>
+    <s v="Ryan Lawton"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="4858.45"/>
+    <n v="498.27"/>
+    <n v="4360.18"/>
+  </r>
+  <r>
+    <s v="Samuel Kackowski"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="2617.73"/>
+    <n v="230.49"/>
+    <n v="2387.2399999999998"/>
+  </r>
+  <r>
+    <s v="Sydney Hood"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="1"/>
+    <n v="4321.0600000000004"/>
+    <n v="858.94"/>
+    <n v="3462.1200000000003"/>
+  </r>
+  <r>
+    <s v="Ted Harris"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="1188.99"/>
+    <n v="406.42"/>
+    <n v="782.56999999999994"/>
+  </r>
+  <r>
+    <s v="Trey Wingo"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="2860.02"/>
+    <n v="268.14999999999998"/>
+    <n v="2591.87"/>
+  </r>
+  <r>
+    <s v="Lisa Steinberg"/>
+    <x v="0"/>
+    <x v="3"/>
+    <x v="4"/>
+    <n v="2966.14"/>
+    <n v="515.04999999999995"/>
+    <n v="2451.09"/>
+  </r>
+  <r>
+    <s v="Catherine Williams"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="1717.44"/>
+    <n v="325.81"/>
+    <n v="1391.63"/>
+  </r>
+  <r>
+    <s v="Emily Deschanels"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="1050.78"/>
+    <n v="960.32"/>
+    <n v="90.459999999999923"/>
+  </r>
+  <r>
+    <s v="Lisa Vanderbeck"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="3371.85"/>
+    <n v="555.99"/>
+    <n v="2815.8599999999997"/>
+  </r>
+  <r>
+    <s v="Lori Rukstad"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="4"/>
+    <n v="1186.93"/>
+    <n v="705.79"/>
+    <n v="481.1400000000001"/>
+  </r>
+  <r>
+    <s v="Michael Roberts"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="3020.27"/>
+    <n v="995.32"/>
+    <n v="2024.9499999999998"/>
+  </r>
+  <r>
+    <s v="Peter Little"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="4"/>
+    <n v="3120.05"/>
+    <n v="218.52"/>
+    <n v="2901.53"/>
+  </r>
+  <r>
+    <s v="Robert Mitchells"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="2015.69"/>
+    <n v="537.07000000000005"/>
+    <n v="1478.62"/>
+  </r>
+  <r>
+    <s v="Ryan Lawton"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="2999.39"/>
+    <n v="624.33000000000004"/>
+    <n v="2375.06"/>
+  </r>
+  <r>
+    <s v="Samuel Kackowski"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="4"/>
+    <n v="2788.69"/>
+    <n v="848.7"/>
+    <n v="1939.99"/>
+  </r>
+  <r>
+    <s v="Sydney Hood"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="2603.16"/>
+    <n v="869.14"/>
+    <n v="1734.02"/>
+  </r>
+  <r>
+    <s v="Ted Harris"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="1980.79"/>
+    <n v="253.46"/>
+    <n v="1727.33"/>
+  </r>
+  <r>
+    <s v="Trey Wingo"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="4581.12"/>
+    <n v="460.58"/>
+    <n v="4120.54"/>
+  </r>
+  <r>
+    <s v="Lisa Steinberg"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="3"/>
+    <n v="2763.03"/>
+    <n v="684.94"/>
+    <n v="2078.09"/>
+  </r>
+  <r>
+    <s v="Catherine Williams"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="4872.05"/>
+    <n v="449.08"/>
+    <n v="4422.97"/>
+  </r>
+  <r>
+    <s v="Emily Deschanels"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="4251.6099999999997"/>
+    <n v="971.83"/>
+    <n v="3279.7799999999997"/>
+  </r>
+  <r>
+    <s v="Lisa Vanderbeck"/>
+    <x v="0"/>
+    <x v="3"/>
+    <x v="4"/>
+    <n v="1436.72"/>
+    <n v="854.32"/>
+    <n v="582.4"/>
+  </r>
+  <r>
+    <s v="Lori Rukstad"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="3932.23"/>
+    <n v="590.98"/>
+    <n v="3341.25"/>
+  </r>
+  <r>
+    <s v="Michael Roberts"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="3025.03"/>
+    <n v="400.12"/>
+    <n v="2624.9100000000003"/>
+  </r>
+  <r>
+    <s v="Peter Little"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="4781.57"/>
+    <n v="347.87"/>
+    <n v="4433.7"/>
+  </r>
+  <r>
+    <s v="Robert Mitchells"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="1483.14"/>
+    <n v="725.89"/>
+    <n v="757.25000000000011"/>
+  </r>
+  <r>
+    <s v="Ryan Lawton"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="1184.5899999999999"/>
+    <n v="405.99"/>
+    <n v="778.59999999999991"/>
+  </r>
+  <r>
+    <s v="Samuel Kackowski"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="3"/>
+    <n v="4370.37"/>
+    <n v="391.49"/>
+    <n v="3978.88"/>
+  </r>
+  <r>
+    <s v="Sydney Hood"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="2496.0700000000002"/>
+    <n v="606.55999999999995"/>
+    <n v="1889.5100000000002"/>
+  </r>
+  <r>
+    <s v="Ted Harris"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="1565.46"/>
+    <n v="625.16"/>
+    <n v="940.30000000000007"/>
+  </r>
+  <r>
+    <s v="Trey Wingo"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="4275.7299999999996"/>
+    <n v="797.13"/>
+    <n v="3478.5999999999995"/>
+  </r>
+  <r>
+    <s v="Lisa Steinberg"/>
+    <x v="0"/>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="1938.91"/>
+    <n v="772.46"/>
+    <n v="1166.45"/>
+  </r>
+  <r>
+    <s v="Catherine Williams"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="4"/>
+    <n v="4019.97"/>
+    <n v="907.81"/>
+    <n v="3112.16"/>
+  </r>
+  <r>
+    <s v="Emily Deschanels"/>
+    <x v="0"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="2261.56"/>
+    <n v="488.04"/>
+    <n v="1773.52"/>
+  </r>
+  <r>
+    <s v="Lisa Vanderbeck"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="4428.54"/>
+    <n v="984"/>
+    <n v="3444.54"/>
+  </r>
+  <r>
+    <s v="Lori Rukstad"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="1541.85"/>
+    <n v="918.32"/>
+    <n v="623.52999999999986"/>
+  </r>
+  <r>
+    <s v="Michael Roberts"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="3309.52"/>
+    <n v="799.05"/>
+    <n v="2510.4700000000003"/>
+  </r>
+  <r>
+    <s v="Peter Little"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="3880.7"/>
+    <n v="840.27"/>
+    <n v="3040.43"/>
+  </r>
+  <r>
+    <s v="Robert Mitchells"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="2878.96"/>
+    <n v="816.58"/>
+    <n v="2062.38"/>
+  </r>
+  <r>
+    <s v="Ryan Lawton"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="1400.81"/>
+    <n v="442.08"/>
+    <n v="958.73"/>
+  </r>
+  <r>
+    <s v="Samuel Kackowski"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="4"/>
+    <n v="4172.84"/>
+    <n v="836.31"/>
+    <n v="3336.53"/>
+  </r>
+  <r>
+    <s v="Sydney Hood"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="4121.7299999999996"/>
+    <n v="228.54"/>
+    <n v="3893.1899999999996"/>
+  </r>
+  <r>
+    <s v="Ted Harris"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="4"/>
+    <n v="4017.37"/>
+    <n v="879.93"/>
+    <n v="3137.44"/>
+  </r>
+  <r>
+    <s v="Trey Wingo"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="2967.91"/>
+    <n v="396.79"/>
+    <n v="2571.12"/>
+  </r>
+  <r>
+    <s v="Lisa Steinberg"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="1294.95"/>
+    <n v="520.15"/>
+    <n v="774.80000000000007"/>
+  </r>
+  <r>
+    <s v="Catherine Williams"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="2"/>
+    <n v="1210.3699999999999"/>
+    <n v="958.23"/>
+    <n v="252.13999999999987"/>
+  </r>
+  <r>
+    <s v="Emily Deschanels"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="4604.03"/>
+    <n v="929.77"/>
+    <n v="3674.2599999999998"/>
+  </r>
+  <r>
+    <s v="Lisa Vanderbeck"/>
+    <x v="0"/>
+    <x v="3"/>
+    <x v="2"/>
+    <n v="3484.06"/>
+    <n v="781.04"/>
+    <n v="2703.02"/>
+  </r>
+  <r>
+    <s v="Lori Rukstad"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="3627.21"/>
+    <n v="567.72"/>
+    <n v="3059.49"/>
+  </r>
+  <r>
+    <s v="Michael Roberts"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="1824.46"/>
+    <n v="727.39"/>
+    <n v="1097.0700000000002"/>
+  </r>
+  <r>
+    <s v="Peter Little"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="3"/>
+    <n v="1620.43"/>
+    <n v="253.6"/>
+    <n v="1366.8300000000002"/>
+  </r>
+  <r>
+    <s v="Robert Mitchells"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="3"/>
+    <n v="1042.29"/>
+    <n v="916.83"/>
+    <n v="125.45999999999992"/>
+  </r>
+  <r>
+    <s v="Ryan Lawton"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="4446.9799999999996"/>
+    <n v="957.43"/>
+    <n v="3489.5499999999997"/>
+  </r>
+  <r>
+    <s v="Samuel Kackowski"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="1"/>
+    <n v="3815.47"/>
+    <n v="263.14999999999998"/>
+    <n v="3552.3199999999997"/>
+  </r>
+  <r>
+    <s v="Sydney Hood"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="4"/>
+    <n v="2619.39"/>
+    <n v="562.27"/>
+    <n v="2057.12"/>
+  </r>
+  <r>
+    <s v="Ted Harris"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="1"/>
+    <n v="4418.3900000000003"/>
+    <n v="335.14"/>
+    <n v="4083.2500000000005"/>
+  </r>
+  <r>
+    <s v="Trey Wingo"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="1410.52"/>
+    <n v="395.64"/>
+    <n v="1014.88"/>
+  </r>
+  <r>
+    <s v="Lisa Steinberg"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="1450.87"/>
+    <n v="376.88"/>
+    <n v="1073.9899999999998"/>
+  </r>
+  <r>
+    <s v="Catherine Williams"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="2609.6999999999998"/>
+    <n v="710.14"/>
+    <n v="1899.56"/>
+  </r>
+  <r>
+    <s v="Emily Deschanels"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="1056.3800000000001"/>
+    <n v="950.68"/>
+    <n v="105.70000000000016"/>
+  </r>
+  <r>
+    <s v="Lisa Vanderbeck"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="4"/>
+    <n v="2192.8200000000002"/>
+    <n v="765"/>
+    <n v="1427.8200000000002"/>
+  </r>
+  <r>
+    <s v="Lori Rukstad"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="3"/>
+    <n v="1055.1300000000001"/>
+    <n v="323.56"/>
+    <n v="731.57000000000016"/>
+  </r>
+  <r>
+    <s v="Michael Roberts"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="4757.45"/>
+    <n v="933.11"/>
+    <n v="3824.3399999999997"/>
+  </r>
+  <r>
+    <s v="Peter Little"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="3870.79"/>
+    <n v="252.64"/>
+    <n v="3618.15"/>
+  </r>
+  <r>
+    <s v="Robert Mitchells"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="2"/>
+    <n v="4812.6899999999996"/>
+    <n v="303.8"/>
+    <n v="4508.8899999999994"/>
+  </r>
+  <r>
+    <s v="Ryan Lawton"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="4077.52"/>
+    <n v="410.78"/>
+    <n v="3666.74"/>
+  </r>
+  <r>
+    <s v="Samuel Kackowski"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="3335.8"/>
+    <n v="452.2"/>
+    <n v="2883.6000000000004"/>
+  </r>
+  <r>
+    <s v="Sydney Hood"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="3518.97"/>
+    <n v="410.01"/>
+    <n v="3108.96"/>
+  </r>
+  <r>
+    <s v="Ted Harris"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="3331.45"/>
+    <n v="850.83"/>
+    <n v="2480.62"/>
+  </r>
+  <r>
+    <s v="Trey Wingo"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="3"/>
+    <n v="4473.34"/>
+    <n v="915.43"/>
+    <n v="3557.9100000000003"/>
+  </r>
+  <r>
+    <s v="Lisa Steinberg"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="4470.66"/>
+    <n v="938.23"/>
+    <n v="3532.43"/>
+  </r>
+  <r>
+    <s v="Catherine Williams"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="1"/>
+    <n v="3384.99"/>
+    <n v="821.1"/>
+    <n v="2563.89"/>
+  </r>
+  <r>
+    <s v="Emily Deschanels"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="4"/>
+    <n v="1870.71"/>
+    <n v="945.17"/>
+    <n v="925.54000000000008"/>
+  </r>
+  <r>
+    <s v="Lisa Vanderbeck"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="4764.0200000000004"/>
+    <n v="304.26"/>
+    <n v="4459.76"/>
+  </r>
+  <r>
+    <s v="Lori Rukstad"/>
+    <x v="0"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="4092.66"/>
+    <n v="671.1"/>
+    <n v="3421.56"/>
+  </r>
+  <r>
+    <s v="Michael Roberts"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="4"/>
+    <n v="2480.86"/>
+    <n v="428.45"/>
+    <n v="2052.4100000000003"/>
+  </r>
+  <r>
+    <s v="Peter Little"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="3811.66"/>
+    <n v="348.63"/>
+    <n v="3463.0299999999997"/>
+  </r>
+  <r>
+    <s v="Robert Mitchells"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="3650.14"/>
+    <n v="851.42"/>
+    <n v="2798.72"/>
+  </r>
+  <r>
+    <s v="Ryan Lawton"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="2625.52"/>
+    <n v="720.71"/>
+    <n v="1904.81"/>
+  </r>
+  <r>
+    <s v="Samuel Kackowski"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="4"/>
+    <n v="1375.5"/>
+    <n v="927.44"/>
+    <n v="448.05999999999995"/>
+  </r>
+  <r>
+    <s v="Sydney Hood"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="1293.67"/>
+    <n v="598.72"/>
+    <n v="694.95"/>
+  </r>
+  <r>
+    <s v="Ted Harris"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="3639.91"/>
+    <n v="316.81"/>
+    <n v="3323.1"/>
+  </r>
+  <r>
+    <s v="Trey Wingo"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="3147.57"/>
+    <n v="645.65"/>
+    <n v="2501.92"/>
+  </r>
+  <r>
+    <s v="Lisa Steinberg"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="2355.9699999999998"/>
+    <n v="502.45"/>
+    <n v="1853.5199999999998"/>
+  </r>
+  <r>
+    <s v="Catherine Williams"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="1694.13"/>
+    <n v="737.33"/>
+    <n v="956.80000000000007"/>
+  </r>
+  <r>
+    <s v="Emily Deschanels"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="1978.86"/>
+    <n v="653.24"/>
+    <n v="1325.62"/>
+  </r>
+  <r>
+    <s v="Lisa Vanderbeck"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="2419.64"/>
+    <n v="904.22"/>
+    <n v="1515.4199999999998"/>
+  </r>
+  <r>
+    <s v="Lori Rukstad"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="2889.26"/>
+    <n v="585.16999999999996"/>
+    <n v="2304.09"/>
+  </r>
+  <r>
+    <s v="Michael Roberts"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="3064.33"/>
+    <n v="374.15"/>
+    <n v="2690.18"/>
+  </r>
+  <r>
+    <s v="Peter Little"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="2321.86"/>
+    <n v="599.69000000000005"/>
+    <n v="1722.17"/>
+  </r>
+  <r>
+    <s v="Robert Mitchells"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="4062.94"/>
+    <n v="346.39"/>
+    <n v="3716.55"/>
+  </r>
+  <r>
+    <s v="Ryan Lawton"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="4"/>
+    <n v="1667.16"/>
+    <n v="273.61"/>
+    <n v="1393.5500000000002"/>
+  </r>
+  <r>
+    <s v="Samuel Kackowski"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="2369.5700000000002"/>
+    <n v="328.16"/>
+    <n v="2041.41"/>
+  </r>
+  <r>
+    <s v="Sydney Hood"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="4765.7700000000004"/>
+    <n v="388.99"/>
+    <n v="4376.7800000000007"/>
+  </r>
+  <r>
+    <s v="Ted Harris"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="3578.96"/>
+    <n v="362.42"/>
+    <n v="3216.54"/>
+  </r>
+  <r>
+    <s v="Trey Wingo"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="3317.29"/>
+    <n v="791.55"/>
+    <n v="2525.7399999999998"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:F8" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="7">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="5">
+        <item x="1"/>
+        <item x="0"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="6">
+        <item h="1" x="0"/>
+        <item x="2"/>
+        <item h="1" x="1"/>
+        <item h="1" x="4"/>
+        <item h="1" x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="167" showAll="0"/>
+    <pivotField dataField="1" numFmtId="164" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="2"/>
+  </colFields>
+  <colItems count="5">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="3" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Sum of Profit" fld="6" baseField="0" baseItem="0" numFmtId="164"/>
+  </dataFields>
+  <formats count="3">
+    <format dxfId="4">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="3">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="0">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3874,7 +6030,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3885,28 +6041,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="23" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
     </row>
     <row r="2" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="47" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
     </row>
     <row r="3" spans="1:8" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -3947,23 +6103,23 @@
       <c r="A7" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="39">
+      <c r="B7" s="33">
         <v>236200</v>
       </c>
-      <c r="C7" s="39">
+      <c r="C7" s="33">
         <v>307060</v>
       </c>
-      <c r="D7" s="39">
+      <c r="D7" s="33">
         <v>347214</v>
       </c>
-      <c r="E7" s="39">
+      <c r="E7" s="33">
         <v>229114</v>
       </c>
-      <c r="F7" s="40">
+      <c r="F7" s="34">
         <f>SUM(B7:E7)</f>
         <v>1119588</v>
       </c>
-      <c r="G7" s="40">
+      <c r="G7" s="34">
         <f>F7*$B$4</f>
         <v>335876.39999999997</v>
       </c>
@@ -3973,24 +6129,24 @@
       <c r="A8" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="39">
+      <c r="B8" s="33">
         <v>522300</v>
       </c>
-      <c r="C8" s="39">
+      <c r="C8" s="33">
         <v>578990</v>
       </c>
-      <c r="D8" s="39">
+      <c r="D8" s="33">
         <v>767781</v>
       </c>
-      <c r="E8" s="39">
+      <c r="E8" s="33">
         <v>578411</v>
       </c>
-      <c r="F8" s="40">
-        <f t="shared" ref="F8:F11" si="0">SUM(B8:E8)</f>
+      <c r="F8" s="34">
+        <f>SUM(B8:E8)</f>
         <v>2447482</v>
       </c>
-      <c r="G8" s="40">
-        <f t="shared" ref="G8:G11" si="1">F8*$B$4</f>
+      <c r="G8" s="34">
+        <f>F8*$B$4</f>
         <v>734244.6</v>
       </c>
       <c r="H8" s="23"/>
@@ -3999,24 +6155,24 @@
       <c r="A9" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="39">
+      <c r="B9" s="33">
         <v>487200</v>
       </c>
-      <c r="C9" s="39">
+      <c r="C9" s="33">
         <v>633660</v>
       </c>
-      <c r="D9" s="39">
+      <c r="D9" s="33">
         <v>501314</v>
       </c>
-      <c r="E9" s="39">
+      <c r="E9" s="33">
         <v>564555</v>
       </c>
-      <c r="F9" s="40">
-        <f t="shared" si="0"/>
+      <c r="F9" s="34">
+        <f>SUM(B9:E9)</f>
         <v>2186729</v>
       </c>
-      <c r="G9" s="40">
-        <f t="shared" si="1"/>
+      <c r="G9" s="34">
+        <f>F9*$B$4</f>
         <v>656018.69999999995</v>
       </c>
       <c r="H9" s="23"/>
@@ -4025,24 +6181,24 @@
       <c r="A10" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="39">
+      <c r="B10" s="33">
         <v>625112</v>
       </c>
-      <c r="C10" s="39">
+      <c r="C10" s="33">
         <v>812645</v>
       </c>
-      <c r="D10" s="39">
+      <c r="D10" s="33">
         <v>918945</v>
       </c>
-      <c r="E10" s="39">
+      <c r="E10" s="33">
         <v>606332</v>
       </c>
-      <c r="F10" s="40">
-        <f t="shared" si="0"/>
+      <c r="F10" s="34">
+        <f>SUM(B10:E10)</f>
         <v>2963034</v>
       </c>
-      <c r="G10" s="40">
-        <f t="shared" si="1"/>
+      <c r="G10" s="34">
+        <f>F10*$B$4</f>
         <v>888910.2</v>
       </c>
       <c r="H10" s="23"/>
@@ -4051,24 +6207,24 @@
       <c r="A11" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="39">
+      <c r="B11" s="33">
         <v>152622</v>
       </c>
-      <c r="C11" s="39">
+      <c r="C11" s="33">
         <v>198408</v>
       </c>
-      <c r="D11" s="39">
+      <c r="D11" s="33">
         <v>155694</v>
       </c>
-      <c r="E11" s="39">
+      <c r="E11" s="33">
         <v>148022</v>
       </c>
-      <c r="F11" s="40">
-        <f t="shared" si="0"/>
+      <c r="F11" s="34">
+        <f>SUM(B11:E11)</f>
         <v>654746</v>
       </c>
-      <c r="G11" s="40">
-        <f t="shared" si="1"/>
+      <c r="G11" s="34">
+        <f>F11*$B$4</f>
         <v>196423.8</v>
       </c>
       <c r="H11" s="23"/>
@@ -4077,28 +6233,28 @@
       <c r="A12" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="41">
-        <f t="shared" ref="B12:G12" si="2">SUM(B7:B11)</f>
+      <c r="B12" s="35">
+        <f t="shared" ref="B12:G12" si="0">SUM(B7:B11)</f>
         <v>2023434</v>
       </c>
-      <c r="C12" s="41">
-        <f t="shared" si="2"/>
+      <c r="C12" s="35">
+        <f t="shared" si="0"/>
         <v>2530763</v>
       </c>
-      <c r="D12" s="41">
-        <f t="shared" si="2"/>
+      <c r="D12" s="35">
+        <f t="shared" si="0"/>
         <v>2690948</v>
       </c>
-      <c r="E12" s="41">
-        <f t="shared" si="2"/>
+      <c r="E12" s="35">
+        <f t="shared" si="0"/>
         <v>2126434</v>
       </c>
-      <c r="F12" s="41">
-        <f t="shared" si="2"/>
+      <c r="F12" s="35">
+        <f t="shared" si="0"/>
         <v>9371579</v>
       </c>
-      <c r="G12" s="41">
-        <f t="shared" si="2"/>
+      <c r="G12" s="35">
+        <f t="shared" si="0"/>
         <v>2811473.6999999997</v>
       </c>
       <c r="H12" s="26"/>
@@ -4174,45 +6330,49 @@
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="N46" sqref="N46"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.1640625" customWidth="1"/>
     <col min="2" max="2" width="9.1640625" customWidth="1"/>
-    <col min="3" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.1640625" customWidth="1"/>
+    <col min="4" max="4" width="14.5" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" customWidth="1"/>
+    <col min="6" max="6" width="14.1640625" customWidth="1"/>
+    <col min="7" max="7" width="15.5" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
     <col min="9" max="11" width="9.1640625" customWidth="1"/>
+    <col min="13" max="13" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="23" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
       <c r="I1" s="18"/>
       <c r="J1" s="18"/>
     </row>
     <row r="2" spans="1:10" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="49" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
     </row>
     <row r="3" spans="1:10" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="E3" s="6"/>
@@ -4254,19 +6414,19 @@
       <c r="B5" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C5" s="43">
+      <c r="C5" s="39">
         <v>18638.333333333332</v>
       </c>
-      <c r="D5" s="43">
+      <c r="D5" s="39">
         <v>24229.833333333332</v>
       </c>
-      <c r="E5" s="43">
+      <c r="E5" s="39">
         <v>25586.704000000002</v>
       </c>
-      <c r="F5" s="43">
+      <c r="F5" s="39">
         <v>17398.958720000002</v>
       </c>
-      <c r="G5" s="43">
+      <c r="G5" s="42">
         <f>SUM(C5:F5)</f>
         <v>85853.829386666679</v>
       </c>
@@ -4282,20 +6442,20 @@
       <c r="B6" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="44">
+      <c r="C6" s="40">
         <v>21185</v>
       </c>
-      <c r="D6" s="44">
+      <c r="D6" s="40">
         <v>21167</v>
       </c>
-      <c r="E6" s="44">
+      <c r="E6" s="40">
         <v>28884</v>
       </c>
-      <c r="F6" s="44">
+      <c r="F6" s="40">
         <v>21875</v>
       </c>
-      <c r="G6" s="43">
-        <f t="shared" ref="G6:G17" si="0">SUM(C6:F6)</f>
+      <c r="G6" s="42">
+        <f t="shared" ref="G6:G16" si="0">SUM(C6:F6)</f>
         <v>93111</v>
       </c>
       <c r="H6" s="5" t="str">
@@ -4310,19 +6470,19 @@
       <c r="B7" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C7" s="44">
+      <c r="C7" s="40">
         <v>19603</v>
       </c>
-      <c r="D7" s="44">
+      <c r="D7" s="40">
         <v>13467</v>
       </c>
-      <c r="E7" s="44">
+      <c r="E7" s="40">
         <v>28363</v>
       </c>
-      <c r="F7" s="44">
+      <c r="F7" s="40">
         <v>18703</v>
       </c>
-      <c r="G7" s="43">
+      <c r="G7" s="42">
         <f t="shared" si="0"/>
         <v>80136</v>
       </c>
@@ -4338,19 +6498,19 @@
       <c r="B8" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="44">
+      <c r="C8" s="40">
         <v>18786.555555555555</v>
       </c>
-      <c r="D8" s="44">
+      <c r="D8" s="40">
         <v>24422.522222222222</v>
       </c>
-      <c r="E8" s="44">
+      <c r="E8" s="40">
         <v>25790.183466666669</v>
       </c>
-      <c r="F8" s="44">
+      <c r="F8" s="40">
         <v>17537.324757333336</v>
       </c>
-      <c r="G8" s="43">
+      <c r="G8" s="42">
         <f t="shared" si="0"/>
         <v>86536.586001777774</v>
       </c>
@@ -4366,19 +6526,19 @@
       <c r="B9" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="44">
+      <c r="C9" s="40">
         <v>23425</v>
       </c>
-      <c r="D9" s="44">
+      <c r="D9" s="40">
         <v>30452.5</v>
       </c>
-      <c r="E9" s="44">
+      <c r="E9" s="40">
         <v>32157.84</v>
       </c>
-      <c r="F9" s="44">
+      <c r="F9" s="40">
         <v>21867.331200000001</v>
       </c>
-      <c r="G9" s="43">
+      <c r="G9" s="42">
         <f t="shared" si="0"/>
         <v>107902.6712</v>
       </c>
@@ -4394,19 +6554,19 @@
       <c r="B10" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="44">
+      <c r="C10" s="40">
         <v>26764</v>
       </c>
-      <c r="D10" s="44">
+      <c r="D10" s="40">
         <v>19993</v>
       </c>
-      <c r="E10" s="44">
+      <c r="E10" s="40">
         <v>26398</v>
       </c>
-      <c r="F10" s="44">
+      <c r="F10" s="40">
         <v>19684</v>
       </c>
-      <c r="G10" s="43">
+      <c r="G10" s="42">
         <f t="shared" si="0"/>
         <v>92839</v>
       </c>
@@ -4422,19 +6582,19 @@
       <c r="B11" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="44">
+      <c r="C11" s="40">
         <v>28683</v>
       </c>
-      <c r="D11" s="44">
+      <c r="D11" s="40">
         <v>31968</v>
       </c>
-      <c r="E11" s="44">
+      <c r="E11" s="40">
         <v>32958</v>
       </c>
-      <c r="F11" s="44">
+      <c r="F11" s="40">
         <v>11836</v>
       </c>
-      <c r="G11" s="43">
+      <c r="G11" s="42">
         <f t="shared" si="0"/>
         <v>105445</v>
       </c>
@@ -4450,19 +6610,19 @@
       <c r="B12" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="44">
+      <c r="C12" s="40">
         <v>16847</v>
       </c>
-      <c r="D12" s="44">
+      <c r="D12" s="40">
         <v>18693</v>
       </c>
-      <c r="E12" s="44">
+      <c r="E12" s="40">
         <v>18269</v>
       </c>
-      <c r="F12" s="44">
+      <c r="F12" s="40">
         <v>17986</v>
       </c>
-      <c r="G12" s="43">
+      <c r="G12" s="42">
         <f t="shared" si="0"/>
         <v>71795</v>
       </c>
@@ -4478,19 +6638,19 @@
       <c r="B13" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="44">
+      <c r="C13" s="40">
         <v>25203.142857142855</v>
       </c>
-      <c r="D13" s="44">
+      <c r="D13" s="40">
         <v>32600</v>
       </c>
-      <c r="E13" s="44">
+      <c r="E13" s="40">
         <v>34930</v>
       </c>
-      <c r="F13" s="44">
+      <c r="F13" s="40">
         <v>23752.400000000001</v>
       </c>
-      <c r="G13" s="43">
+      <c r="G13" s="42">
         <f t="shared" si="0"/>
         <v>116485.54285714286</v>
       </c>
@@ -4506,19 +6666,19 @@
       <c r="B14" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="44">
+      <c r="C14" s="40">
         <v>18688.947368421053</v>
       </c>
-      <c r="D14" s="44">
+      <c r="D14" s="40">
         <v>24295.63157894737</v>
       </c>
-      <c r="E14" s="44">
+      <c r="E14" s="40">
         <v>25656.186947368424</v>
       </c>
-      <c r="F14" s="44">
+      <c r="F14" s="40">
         <v>17446.20712421053</v>
       </c>
-      <c r="G14" s="43">
+      <c r="G14" s="42">
         <f t="shared" si="0"/>
         <v>86086.973018947378</v>
       </c>
@@ -4534,19 +6694,19 @@
       <c r="B15" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="44">
+      <c r="C15" s="40">
         <v>18747.894736842103</v>
       </c>
-      <c r="D15" s="44">
+      <c r="D15" s="40">
         <v>24372.263157894737</v>
       </c>
-      <c r="E15" s="44">
+      <c r="E15" s="40">
         <v>25737.109894736845</v>
       </c>
-      <c r="F15" s="44">
+      <c r="F15" s="40">
         <v>17501.234728421055</v>
       </c>
-      <c r="G15" s="43">
+      <c r="G15" s="42">
         <f t="shared" si="0"/>
         <v>86358.50251789474</v>
       </c>
@@ -4562,19 +6722,19 @@
       <c r="B16" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="44">
+      <c r="C16" s="40">
         <v>26636</v>
       </c>
-      <c r="D16" s="44">
+      <c r="D16" s="40">
         <v>34626.800000000003</v>
       </c>
-      <c r="E16" s="44">
+      <c r="E16" s="40">
         <v>36565.900800000003</v>
       </c>
-      <c r="F16" s="44">
+      <c r="F16" s="40">
         <v>24864.812544000004</v>
       </c>
-      <c r="G16" s="43">
+      <c r="G16" s="42">
         <f t="shared" si="0"/>
         <v>122693.51334400001</v>
       </c>
@@ -4590,19 +6750,19 @@
       <c r="B17" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="44">
+      <c r="C17" s="40">
         <v>23498</v>
       </c>
-      <c r="D17" s="44">
+      <c r="D17" s="40">
         <v>26597</v>
       </c>
-      <c r="E17" s="44">
+      <c r="E17" s="40">
         <v>28086.432000000001</v>
       </c>
-      <c r="F17" s="44">
+      <c r="F17" s="40">
         <v>22111</v>
       </c>
-      <c r="G17" s="43">
+      <c r="G17" s="42">
         <f>SUM(C17:F17)</f>
         <v>100292.432</v>
       </c>
@@ -4616,24 +6776,24 @@
         <v>0</v>
       </c>
       <c r="B18" s="20"/>
-      <c r="C18" s="45">
+      <c r="C18" s="41">
         <f>SUM(C5:C17)</f>
         <v>286705.87385129486</v>
       </c>
-      <c r="D18" s="45">
-        <f t="shared" ref="D18:G18" si="2">SUM(D5:D17)</f>
+      <c r="D18" s="41">
+        <f>SUM(D5:D17)</f>
         <v>326884.55029239762</v>
       </c>
-      <c r="E18" s="45">
-        <f t="shared" si="2"/>
+      <c r="E18" s="41">
+        <f>SUM(E5:E17)</f>
         <v>369382.35710877192</v>
       </c>
-      <c r="F18" s="45">
-        <f t="shared" si="2"/>
+      <c r="F18" s="41">
+        <f>SUM(F5:F17)</f>
         <v>252563.26907396491</v>
       </c>
-      <c r="G18" s="45">
-        <f t="shared" si="2"/>
+      <c r="G18" s="41">
+        <f>SUM(G5:G17)</f>
         <v>1235536.0503264295</v>
       </c>
       <c r="H18" s="20"/>
@@ -4704,7 +6864,7 @@
         <v>35</v>
       </c>
       <c r="C24" s="7"/>
-      <c r="D24" s="42">
+      <c r="D24" s="34">
         <f>MAX(G5:G17)</f>
         <v>122693.51334400001</v>
       </c>
@@ -4720,9 +6880,9 @@
         <v>36</v>
       </c>
       <c r="C25" s="7"/>
-      <c r="D25" s="38" t="e">
-        <f>VLOOKUP(D24,A5:G17,1,FALSE)</f>
-        <v>#N/A</v>
+      <c r="D25" s="43" t="str">
+        <f>INDEX(A5:A17,MATCH(D24,G5:G17))</f>
+        <v>Ted Harris</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
@@ -4736,7 +6896,7 @@
         <v>37</v>
       </c>
       <c r="C26" s="7"/>
-      <c r="D26" s="17">
+      <c r="D26" s="34">
         <f>MIN(G5:G17)</f>
         <v>71795</v>
       </c>
@@ -4752,9 +6912,9 @@
         <v>38</v>
       </c>
       <c r="C27" s="7"/>
-      <c r="D27" s="17" t="e">
-        <f>VLOOKUP(D26,A5:G17,1,FALSE)</f>
-        <v>#N/A</v>
+      <c r="D27" s="17" t="str">
+        <f>A12</f>
+        <v>Robert Mitchells</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
@@ -4802,7 +6962,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:H17">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",H5)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4838,34 +6998,38 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="28.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="13.1640625" customWidth="1"/>
+    <col min="2" max="2" width="15.1640625" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" customWidth="1"/>
+    <col min="4" max="4" width="16.83203125" customWidth="1"/>
+    <col min="5" max="5" width="16.1640625" customWidth="1"/>
+    <col min="6" max="6" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
     </row>
     <row r="2" spans="1:6" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="47" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
     </row>
     <row r="3" spans="1:6" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -4900,23 +7064,23 @@
       <c r="A7" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="39">
+      <c r="B7" s="28">
         <f>'Quarterly Sales Summary'!$F$7</f>
         <v>1119588</v>
       </c>
-      <c r="C7" s="49">
+      <c r="C7" s="37">
         <f>B7/B$12</f>
         <v>0.11946631405444055</v>
       </c>
-      <c r="D7" s="37">
+      <c r="D7" s="28">
         <f>B7*($B$4+100%)</f>
         <v>1455464.4000000001</v>
       </c>
-      <c r="E7" s="50">
+      <c r="E7" s="28">
         <f>D7</f>
         <v>1455464.4000000001</v>
       </c>
-      <c r="F7" s="48">
+      <c r="F7" s="36">
         <f>E7/E$12</f>
         <v>0.10917934892195989</v>
       </c>
@@ -4925,24 +7089,24 @@
       <c r="A8" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="46">
+      <c r="B8" s="28">
         <f>'Quarterly Sales Summary'!$F$8</f>
         <v>2447482</v>
       </c>
-      <c r="C8" s="49">
-        <f t="shared" ref="C8:C11" si="0">B8/B$12</f>
+      <c r="C8" s="37">
+        <f>B8/B$12</f>
         <v>0.26116004570841261</v>
       </c>
-      <c r="D8" s="51">
+      <c r="D8" s="28">
         <f>B8*($B$4+100%)</f>
         <v>3181726.6</v>
       </c>
-      <c r="E8" s="50">
-        <f t="shared" ref="E8:E10" si="1">D8</f>
+      <c r="E8" s="28">
+        <f>D8</f>
         <v>3181726.6</v>
       </c>
-      <c r="F8" s="48">
-        <f t="shared" ref="F8:F11" si="2">E8/E$12</f>
+      <c r="F8" s="36">
+        <f>E8/E$12</f>
         <v>0.23867216445533199</v>
       </c>
     </row>
@@ -4950,24 +7114,24 @@
       <c r="A9" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="46">
+      <c r="B9" s="28">
         <f>'Quarterly Sales Summary'!$F$9</f>
         <v>2186729</v>
       </c>
-      <c r="C9" s="49">
-        <f t="shared" si="0"/>
+      <c r="C9" s="37">
+        <f>B9/B$12</f>
         <v>0.23333623928262248</v>
       </c>
-      <c r="D9" s="51">
+      <c r="D9" s="28">
         <f>B9*($B$4+100%)</f>
         <v>2842747.7</v>
       </c>
-      <c r="E9" s="50">
-        <f t="shared" si="1"/>
+      <c r="E9" s="28">
+        <f>D9</f>
         <v>2842747.7</v>
       </c>
-      <c r="F9" s="48">
-        <f t="shared" si="2"/>
+      <c r="F9" s="36">
+        <f>E9/E$12</f>
         <v>0.21324420098176153</v>
       </c>
     </row>
@@ -4975,24 +7139,24 @@
       <c r="A10" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="46">
+      <c r="B10" s="28">
         <f>'Quarterly Sales Summary'!$F$10</f>
         <v>2963034</v>
       </c>
-      <c r="C10" s="49">
-        <f t="shared" si="0"/>
+      <c r="C10" s="37">
+        <f>B10/B$12</f>
         <v>0.31617233339227041</v>
       </c>
-      <c r="D10" s="51">
+      <c r="D10" s="28">
         <f>B10*($B$4+100%)</f>
         <v>3851944.2</v>
       </c>
-      <c r="E10" s="50">
-        <f t="shared" si="1"/>
+      <c r="E10" s="28">
+        <f>D10</f>
         <v>3851944.2</v>
       </c>
-      <c r="F10" s="48">
-        <f t="shared" si="2"/>
+      <c r="F10" s="36">
+        <f>E10/E$12</f>
         <v>0.28894747260030523</v>
       </c>
     </row>
@@ -5000,23 +7164,23 @@
       <c r="A11" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="46">
+      <c r="B11" s="28">
         <f>'Quarterly Sales Summary'!$F$11</f>
         <v>654746</v>
       </c>
-      <c r="C11" s="49">
-        <f t="shared" si="0"/>
+      <c r="C11" s="37">
+        <f>B11/B$12</f>
         <v>6.9865067562253913E-2</v>
       </c>
-      <c r="D11" s="51">
+      <c r="D11" s="28">
         <f>B11*($B$4+100%)</f>
         <v>851169.8</v>
       </c>
-      <c r="E11" s="50">
+      <c r="E11" s="28">
         <v>1999066.7197888931</v>
       </c>
       <c r="F11" s="32">
-        <f t="shared" si="2"/>
+        <f>E11/E$12</f>
         <v>0.14995681304064146</v>
       </c>
     </row>
@@ -5024,16 +7188,16 @@
       <c r="A12" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="47">
+      <c r="B12" s="44">
         <f>SUM(B7:B11)</f>
         <v>9371579</v>
       </c>
       <c r="C12" s="24"/>
-      <c r="D12" s="52">
+      <c r="D12" s="44">
         <f>SUM(D7:D11)</f>
         <v>12183052.700000001</v>
       </c>
-      <c r="E12" s="52">
+      <c r="E12" s="44">
         <f>SUM(E7:E11)</f>
         <v>13330949.619788893</v>
       </c>
@@ -5077,13 +7241,149 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.33203125" customWidth="1"/>
+    <col min="2" max="2" width="25.5" customWidth="1"/>
+    <col min="3" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="50" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="50" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="50" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="50" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" s="5">
+        <v>1</v>
+      </c>
+      <c r="C4" s="5">
+        <v>2</v>
+      </c>
+      <c r="D4" s="5">
+        <v>3</v>
+      </c>
+      <c r="E4" s="5">
+        <v>4</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="51" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="52">
+        <v>7114.6299999999983</v>
+      </c>
+      <c r="C5" s="52">
+        <v>2510.4700000000003</v>
+      </c>
+      <c r="D5" s="52">
+        <v>7811.62</v>
+      </c>
+      <c r="E5" s="52">
+        <v>220.57000000000005</v>
+      </c>
+      <c r="F5" s="52">
+        <v>17657.289999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="51" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="52">
+        <v>12417.32</v>
+      </c>
+      <c r="C6" s="52">
+        <v>5559.52</v>
+      </c>
+      <c r="D6" s="52">
+        <v>5622.1299999999992</v>
+      </c>
+      <c r="E6" s="52">
+        <v>7010.01</v>
+      </c>
+      <c r="F6" s="52">
+        <v>30608.980000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="51" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="52">
+        <v>5189</v>
+      </c>
+      <c r="C7" s="52">
+        <v>24810.47</v>
+      </c>
+      <c r="D7" s="52">
+        <v>6235.48</v>
+      </c>
+      <c r="E7" s="52">
+        <v>6973.4699999999993</v>
+      </c>
+      <c r="F7" s="52">
+        <v>43208.42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="45" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" s="25">
+        <v>24720.949999999997</v>
+      </c>
+      <c r="C8" s="25">
+        <v>32880.46</v>
+      </c>
+      <c r="D8" s="25">
+        <v>19669.23</v>
+      </c>
+      <c r="E8" s="25">
+        <v>14204.05</v>
+      </c>
+      <c r="F8" s="25">
+        <v>91474.69</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
   <dimension ref="A1:H219"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:G217"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5098,31 +7398,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="23" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
       <c r="H1" s="18"/>
     </row>
     <row r="2" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="49" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
     </row>
     <row r="3" spans="1:8" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="53">
+      <c r="A4" s="38">
         <v>245617.21</v>
       </c>
       <c r="B4" t="s">
@@ -5130,17 +7430,26 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="23">
+        <v>2690.15</v>
+      </c>
       <c r="B5" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="45" t="s">
+        <v>55</v>
+      </c>
       <c r="B6" s="5" t="s">
         <v>63</v>
       </c>
       <c r="E6" s="28"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
+        <v>66</v>
+      </c>
       <c r="B7" t="s">
         <v>65</v>
       </c>
@@ -10172,6 +12481,7 @@
     <mergeCell ref="A2:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
updated PPIT assignment files
</commit_message>
<xml_diff>
--- a/ITW/u3149399/P2-u3149399-SalesReports.xlsx
+++ b/ITW/u3149399/P2-u3149399-SalesReports.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tenzin/Documents/semester1/assignments/ITW/u3149399/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tenzin/Documents/semester1/assignments/ITW/ITW-2017-S1-A1-u3149399/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Quarterly Sales Summary" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="5" r:id="rId6"/>
+    <pivotCache cacheId="0" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -327,18 +327,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor theme="4" tint="0.79998168889431442"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="7">
@@ -493,7 +487,6 @@
     <xf numFmtId="44" fontId="5" fillId="0" borderId="3" xfId="17" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="16" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="15" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -509,6 +502,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="11" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -521,11 +519,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="10" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="18">
     <cellStyle name="5poRJfl+ZUAkAS/y55FTKjP2V4R9Xff8nrFfXKHIidA=-~DyJpIdC918Oc2CKKuumpPw==" xfId="10"/>
@@ -547,53 +541,9 @@
     <cellStyle name="Title" xfId="11" builtinId="15"/>
     <cellStyle name="Total" xfId="17" builtinId="25"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="4">
     <dxf>
       <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
     </dxf>
     <dxf>
       <border>
@@ -708,7 +658,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1134,11 +1083,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="2123763680"/>
-        <c:axId val="2123768800"/>
+        <c:axId val="2117350880"/>
+        <c:axId val="2117342752"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2123763680"/>
+        <c:axId val="2117350880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1169,7 +1118,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1234,7 +1182,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2123768800"/>
+        <c:crossAx val="2117342752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1242,7 +1190,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2123768800"/>
+        <c:axId val="2117342752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1287,7 +1235,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1346,7 +1293,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2123763680"/>
+        <c:crossAx val="2117350880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1360,7 +1307,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2204,11 +2150,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-24"/>
-        <c:axId val="-2137741104"/>
-        <c:axId val="-2117608704"/>
+        <c:axId val="2117213664"/>
+        <c:axId val="2117207552"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2137741104"/>
+        <c:axId val="2117213664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2304,7 +2250,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2117608704"/>
+        <c:crossAx val="2117207552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2312,7 +2258,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2117608704"/>
+        <c:axId val="2117207552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2415,7 +2361,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2137741104"/>
+        <c:crossAx val="2117213664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5631,7 +5577,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:F8" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -5710,14 +5656,14 @@
     <dataField name="Sum of Profit" fld="6" baseField="0" baseItem="0" numFmtId="164"/>
   </dataFields>
   <formats count="3">
-    <format dxfId="4">
+    <format dxfId="2">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="3">
+    <format dxfId="1">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
@@ -6041,28 +5987,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="23" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
     </row>
     <row r="2" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="47"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
     </row>
     <row r="3" spans="1:8" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -6330,8 +6276,8 @@
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6349,30 +6295,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="23" x14ac:dyDescent="0.25">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
       <c r="I1" s="18"/>
       <c r="J1" s="18"/>
     </row>
     <row r="2" spans="1:10" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
     </row>
     <row r="3" spans="1:10" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="E3" s="6"/>
@@ -6414,19 +6360,19 @@
       <c r="B5" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C5" s="39">
+      <c r="C5" s="38">
         <v>18638.333333333332</v>
       </c>
-      <c r="D5" s="39">
+      <c r="D5" s="38">
         <v>24229.833333333332</v>
       </c>
-      <c r="E5" s="39">
+      <c r="E5" s="38">
         <v>25586.704000000002</v>
       </c>
-      <c r="F5" s="39">
+      <c r="F5" s="38">
         <v>17398.958720000002</v>
       </c>
-      <c r="G5" s="42">
+      <c r="G5" s="41">
         <f>SUM(C5:F5)</f>
         <v>85853.829386666679</v>
       </c>
@@ -6442,19 +6388,19 @@
       <c r="B6" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="40">
+      <c r="C6" s="39">
         <v>21185</v>
       </c>
-      <c r="D6" s="40">
+      <c r="D6" s="39">
         <v>21167</v>
       </c>
-      <c r="E6" s="40">
+      <c r="E6" s="39">
         <v>28884</v>
       </c>
-      <c r="F6" s="40">
+      <c r="F6" s="39">
         <v>21875</v>
       </c>
-      <c r="G6" s="42">
+      <c r="G6" s="41">
         <f t="shared" ref="G6:G16" si="0">SUM(C6:F6)</f>
         <v>93111</v>
       </c>
@@ -6470,19 +6416,19 @@
       <c r="B7" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C7" s="40">
+      <c r="C7" s="39">
         <v>19603</v>
       </c>
-      <c r="D7" s="40">
+      <c r="D7" s="39">
         <v>13467</v>
       </c>
-      <c r="E7" s="40">
+      <c r="E7" s="39">
         <v>28363</v>
       </c>
-      <c r="F7" s="40">
+      <c r="F7" s="39">
         <v>18703</v>
       </c>
-      <c r="G7" s="42">
+      <c r="G7" s="41">
         <f t="shared" si="0"/>
         <v>80136</v>
       </c>
@@ -6498,19 +6444,19 @@
       <c r="B8" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="40">
+      <c r="C8" s="39">
         <v>18786.555555555555</v>
       </c>
-      <c r="D8" s="40">
+      <c r="D8" s="39">
         <v>24422.522222222222</v>
       </c>
-      <c r="E8" s="40">
+      <c r="E8" s="39">
         <v>25790.183466666669</v>
       </c>
-      <c r="F8" s="40">
+      <c r="F8" s="39">
         <v>17537.324757333336</v>
       </c>
-      <c r="G8" s="42">
+      <c r="G8" s="41">
         <f t="shared" si="0"/>
         <v>86536.586001777774</v>
       </c>
@@ -6526,19 +6472,19 @@
       <c r="B9" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="40">
+      <c r="C9" s="39">
         <v>23425</v>
       </c>
-      <c r="D9" s="40">
+      <c r="D9" s="39">
         <v>30452.5</v>
       </c>
-      <c r="E9" s="40">
+      <c r="E9" s="39">
         <v>32157.84</v>
       </c>
-      <c r="F9" s="40">
+      <c r="F9" s="39">
         <v>21867.331200000001</v>
       </c>
-      <c r="G9" s="42">
+      <c r="G9" s="41">
         <f t="shared" si="0"/>
         <v>107902.6712</v>
       </c>
@@ -6554,19 +6500,19 @@
       <c r="B10" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="40">
+      <c r="C10" s="39">
         <v>26764</v>
       </c>
-      <c r="D10" s="40">
+      <c r="D10" s="39">
         <v>19993</v>
       </c>
-      <c r="E10" s="40">
+      <c r="E10" s="39">
         <v>26398</v>
       </c>
-      <c r="F10" s="40">
+      <c r="F10" s="39">
         <v>19684</v>
       </c>
-      <c r="G10" s="42">
+      <c r="G10" s="41">
         <f t="shared" si="0"/>
         <v>92839</v>
       </c>
@@ -6582,19 +6528,19 @@
       <c r="B11" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="40">
+      <c r="C11" s="39">
         <v>28683</v>
       </c>
-      <c r="D11" s="40">
+      <c r="D11" s="39">
         <v>31968</v>
       </c>
-      <c r="E11" s="40">
+      <c r="E11" s="39">
         <v>32958</v>
       </c>
-      <c r="F11" s="40">
+      <c r="F11" s="39">
         <v>11836</v>
       </c>
-      <c r="G11" s="42">
+      <c r="G11" s="41">
         <f t="shared" si="0"/>
         <v>105445</v>
       </c>
@@ -6610,19 +6556,19 @@
       <c r="B12" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="40">
+      <c r="C12" s="39">
         <v>16847</v>
       </c>
-      <c r="D12" s="40">
+      <c r="D12" s="39">
         <v>18693</v>
       </c>
-      <c r="E12" s="40">
+      <c r="E12" s="39">
         <v>18269</v>
       </c>
-      <c r="F12" s="40">
+      <c r="F12" s="39">
         <v>17986</v>
       </c>
-      <c r="G12" s="42">
+      <c r="G12" s="41">
         <f t="shared" si="0"/>
         <v>71795</v>
       </c>
@@ -6638,19 +6584,19 @@
       <c r="B13" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="40">
+      <c r="C13" s="39">
         <v>25203.142857142855</v>
       </c>
-      <c r="D13" s="40">
+      <c r="D13" s="39">
         <v>32600</v>
       </c>
-      <c r="E13" s="40">
+      <c r="E13" s="39">
         <v>34930</v>
       </c>
-      <c r="F13" s="40">
+      <c r="F13" s="39">
         <v>23752.400000000001</v>
       </c>
-      <c r="G13" s="42">
+      <c r="G13" s="41">
         <f t="shared" si="0"/>
         <v>116485.54285714286</v>
       </c>
@@ -6666,19 +6612,19 @@
       <c r="B14" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="40">
+      <c r="C14" s="39">
         <v>18688.947368421053</v>
       </c>
-      <c r="D14" s="40">
+      <c r="D14" s="39">
         <v>24295.63157894737</v>
       </c>
-      <c r="E14" s="40">
+      <c r="E14" s="39">
         <v>25656.186947368424</v>
       </c>
-      <c r="F14" s="40">
+      <c r="F14" s="39">
         <v>17446.20712421053</v>
       </c>
-      <c r="G14" s="42">
+      <c r="G14" s="41">
         <f t="shared" si="0"/>
         <v>86086.973018947378</v>
       </c>
@@ -6694,19 +6640,19 @@
       <c r="B15" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="40">
+      <c r="C15" s="39">
         <v>18747.894736842103</v>
       </c>
-      <c r="D15" s="40">
+      <c r="D15" s="39">
         <v>24372.263157894737</v>
       </c>
-      <c r="E15" s="40">
+      <c r="E15" s="39">
         <v>25737.109894736845</v>
       </c>
-      <c r="F15" s="40">
+      <c r="F15" s="39">
         <v>17501.234728421055</v>
       </c>
-      <c r="G15" s="42">
+      <c r="G15" s="41">
         <f t="shared" si="0"/>
         <v>86358.50251789474</v>
       </c>
@@ -6722,19 +6668,19 @@
       <c r="B16" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="40">
+      <c r="C16" s="39">
         <v>26636</v>
       </c>
-      <c r="D16" s="40">
+      <c r="D16" s="39">
         <v>34626.800000000003</v>
       </c>
-      <c r="E16" s="40">
+      <c r="E16" s="39">
         <v>36565.900800000003</v>
       </c>
-      <c r="F16" s="40">
+      <c r="F16" s="39">
         <v>24864.812544000004</v>
       </c>
-      <c r="G16" s="42">
+      <c r="G16" s="41">
         <f t="shared" si="0"/>
         <v>122693.51334400001</v>
       </c>
@@ -6750,19 +6696,19 @@
       <c r="B17" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="40">
+      <c r="C17" s="39">
         <v>23498</v>
       </c>
-      <c r="D17" s="40">
+      <c r="D17" s="39">
         <v>26597</v>
       </c>
-      <c r="E17" s="40">
+      <c r="E17" s="39">
         <v>28086.432000000001</v>
       </c>
-      <c r="F17" s="40">
+      <c r="F17" s="39">
         <v>22111</v>
       </c>
-      <c r="G17" s="42">
+      <c r="G17" s="41">
         <f>SUM(C17:F17)</f>
         <v>100292.432</v>
       </c>
@@ -6776,23 +6722,23 @@
         <v>0</v>
       </c>
       <c r="B18" s="20"/>
-      <c r="C18" s="41">
+      <c r="C18" s="40">
         <f>SUM(C5:C17)</f>
         <v>286705.87385129486</v>
       </c>
-      <c r="D18" s="41">
+      <c r="D18" s="40">
         <f>SUM(D5:D17)</f>
         <v>326884.55029239762</v>
       </c>
-      <c r="E18" s="41">
+      <c r="E18" s="40">
         <f>SUM(E5:E17)</f>
         <v>369382.35710877192</v>
       </c>
-      <c r="F18" s="41">
+      <c r="F18" s="40">
         <f>SUM(F5:F17)</f>
         <v>252563.26907396491</v>
       </c>
-      <c r="G18" s="41">
+      <c r="G18" s="40">
         <f>SUM(G5:G17)</f>
         <v>1235536.0503264295</v>
       </c>
@@ -6880,7 +6826,7 @@
         <v>36</v>
       </c>
       <c r="C25" s="7"/>
-      <c r="D25" s="43" t="str">
+      <c r="D25" s="42" t="str">
         <f>INDEX(A5:A17,MATCH(D24,G5:G17))</f>
         <v>Ted Harris</v>
       </c>
@@ -6962,7 +6908,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:H17">
-    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",H5)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7012,24 +6958,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23" x14ac:dyDescent="0.25">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
     </row>
     <row r="2" spans="1:6" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="49" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="47"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
     </row>
     <row r="3" spans="1:6" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -7188,16 +7134,16 @@
       <c r="A12" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="44">
+      <c r="B12" s="43">
         <f>SUM(B7:B11)</f>
         <v>9371579</v>
       </c>
       <c r="C12" s="24"/>
-      <c r="D12" s="44">
+      <c r="D12" s="43">
         <f>SUM(D7:D11)</f>
         <v>12183052.700000001</v>
       </c>
-      <c r="E12" s="44">
+      <c r="E12" s="43">
         <f>SUM(E7:E11)</f>
         <v>13330949.619788893</v>
       </c>
@@ -7255,7 +7201,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="45" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="5" t="s">
@@ -7263,15 +7209,15 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="50" t="s">
+      <c r="A3" s="45" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="50" t="s">
+      <c r="B3" s="45" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="50" t="s">
+      <c r="A4" s="45" t="s">
         <v>70</v>
       </c>
       <c r="B4" s="5">
@@ -7291,67 +7237,67 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="51" t="s">
+      <c r="A5" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="52">
+      <c r="B5" s="47">
         <v>7114.6299999999983</v>
       </c>
-      <c r="C5" s="52">
+      <c r="C5" s="47">
         <v>2510.4700000000003</v>
       </c>
-      <c r="D5" s="52">
+      <c r="D5" s="47">
         <v>7811.62</v>
       </c>
-      <c r="E5" s="52">
+      <c r="E5" s="47">
         <v>220.57000000000005</v>
       </c>
-      <c r="F5" s="52">
+      <c r="F5" s="47">
         <v>17657.289999999997</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="51" t="s">
+      <c r="A6" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="52">
+      <c r="B6" s="47">
         <v>12417.32</v>
       </c>
-      <c r="C6" s="52">
+      <c r="C6" s="47">
         <v>5559.52</v>
       </c>
-      <c r="D6" s="52">
+      <c r="D6" s="47">
         <v>5622.1299999999992</v>
       </c>
-      <c r="E6" s="52">
+      <c r="E6" s="47">
         <v>7010.01</v>
       </c>
-      <c r="F6" s="52">
+      <c r="F6" s="47">
         <v>30608.980000000003</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="51" t="s">
+      <c r="A7" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="52">
+      <c r="B7" s="47">
         <v>5189</v>
       </c>
-      <c r="C7" s="52">
+      <c r="C7" s="47">
         <v>24810.47</v>
       </c>
-      <c r="D7" s="52">
+      <c r="D7" s="47">
         <v>6235.48</v>
       </c>
-      <c r="E7" s="52">
+      <c r="E7" s="47">
         <v>6973.4699999999993</v>
       </c>
-      <c r="F7" s="52">
+      <c r="F7" s="47">
         <v>43208.42</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="45" t="s">
+      <c r="A8" s="44" t="s">
         <v>68</v>
       </c>
       <c r="B8" s="25">
@@ -7382,8 +7328,8 @@
   </sheetPr>
   <dimension ref="A1:H219"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:G217"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7398,31 +7344,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="23" x14ac:dyDescent="0.25">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
       <c r="H1" s="18"/>
     </row>
     <row r="2" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="51" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
     </row>
     <row r="3" spans="1:8" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="38">
+      <c r="A4" s="52">
         <v>245617.21</v>
       </c>
       <c r="B4" t="s">
@@ -7438,7 +7384,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="45" t="s">
+      <c r="A6" s="44" t="s">
         <v>55</v>
       </c>
       <c r="B6" s="5" t="s">

</xml_diff>